<commit_message>
Uploading important files from Joplin folder on uFiles. Does not include experiment files yet.
</commit_message>
<xml_diff>
--- a/stim_files/dev_train.xlsx
+++ b/stim_files/dev_train.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/shares/Cabi/exp/joplin/joplin1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Shares/Cabi/exp/joplin/joplin1/stim_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C40F373-09B5-E442-97E8-3F3FF96650C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40326B21-191E-1542-857A-ED9046145DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11800" yWindow="1340" windowWidth="21740" windowHeight="19500" activeTab="8" xr2:uid="{5BDC12A1-80DF-254D-ACB8-0E721CBBF2A6}"/>
+    <workbookView xWindow="11800" yWindow="1340" windowWidth="32540" windowHeight="20120" activeTab="2" xr2:uid="{5BDC12A1-80DF-254D-ACB8-0E721CBBF2A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Set1_7" sheetId="2" r:id="rId2"/>
-    <sheet name="Set2_7" sheetId="7" r:id="rId3"/>
+    <sheet name="Set2_7_THISONE" sheetId="7" r:id="rId3"/>
     <sheet name="Set3_7" sheetId="5" r:id="rId4"/>
     <sheet name="Set 4_5" sheetId="8" r:id="rId5"/>
     <sheet name="Set 5_5" sheetId="10" r:id="rId6"/>
@@ -232,47 +232,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1440,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="L1" t="str">
-        <f t="shared" ref="L1:L35" si="0">A1&amp;B1&amp;C1&amp;D1&amp;E1&amp;F1&amp;G1&amp;H1&amp;I1&amp;J1</f>
+        <f t="shared" ref="L1:L13" si="0">A1&amp;B1&amp;C1&amp;D1&amp;E1&amp;F1&amp;G1&amp;H1&amp;I1&amp;J1</f>
         <v>0100111111</v>
       </c>
     </row>
@@ -1878,39 +1838,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J20">
-    <cfRule type="duplicateValues" dxfId="22" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L21">
-    <cfRule type="duplicateValues" dxfId="21" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:L28">
-    <cfRule type="duplicateValues" dxfId="18" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L28">
-    <cfRule type="duplicateValues" dxfId="15" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L29:L35">
-    <cfRule type="duplicateValues" dxfId="13" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L29:L35">
-    <cfRule type="duplicateValues" dxfId="10" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L35">
-    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L13">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2873,8 +2833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A999D1-EDE6-3D49-9109-1EC371DD7E8C}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:K8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4390,8 +4350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C06F412-CCD8-D642-A63B-6DCB040FD8A7}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>